<commit_message>
life and change atributos armas
</commit_message>
<xml_diff>
--- a/ROGUELIKE/res/armas.xlsx
+++ b/ROGUELIKE/res/armas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cherobin/Documents/Projetos/Apenas-Uma-Vez/ROGUELIKE/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390192A7-46D2-1545-89AC-93F9D79CD8E8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5698BE1A-2DA5-FB44-82CE-46DD251F8526}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="16680" xr2:uid="{A836B3ED-0900-8649-989A-286E2BE47057}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t>imagem</t>
   </si>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>arma 1</t>
-  </si>
-  <si>
-    <t>true</t>
   </si>
   <si>
     <t>arma 2</t>
@@ -472,7 +469,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -484,7 +481,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
         <v>8</v>
@@ -511,10 +508,10 @@
         <v>6</v>
       </c>
       <c r="J1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" t="s">
         <v>28</v>
-      </c>
-      <c r="K1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -528,16 +525,16 @@
         <v>7</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="E2">
-        <v>10</v>
+        <v>200</v>
       </c>
       <c r="F2">
         <v>2000</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -557,22 +554,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="E3">
-        <v>11</v>
+        <v>250</v>
       </c>
       <c r="F3">
         <v>4000</v>
       </c>
       <c r="G3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H3">
         <v>2</v>
@@ -592,22 +589,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>120</v>
       </c>
       <c r="E4">
-        <v>12</v>
+        <v>100</v>
       </c>
       <c r="F4">
         <v>5000</v>
       </c>
       <c r="G4" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="H4">
         <v>3</v>
@@ -627,22 +624,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>200</v>
       </c>
       <c r="E5">
-        <v>13</v>
+        <v>100</v>
       </c>
       <c r="F5">
         <v>6000</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H5">
         <v>4</v>
@@ -662,22 +659,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>1000</v>
       </c>
       <c r="E6">
-        <v>14</v>
+        <v>500</v>
       </c>
       <c r="F6">
         <v>7000</v>
       </c>
       <c r="G6" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="H6">
         <v>5</v>
@@ -697,22 +694,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7">
-        <v>6</v>
+        <v>500</v>
       </c>
       <c r="E7">
-        <v>15</v>
+        <v>150</v>
       </c>
       <c r="F7">
         <v>8000</v>
       </c>
       <c r="G7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H7">
         <v>6</v>
@@ -732,22 +729,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8">
-        <v>7</v>
+        <v>250</v>
       </c>
       <c r="E8">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F8">
         <v>6000</v>
       </c>
       <c r="G8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H8">
         <v>7</v>
@@ -767,22 +764,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9">
-        <v>8</v>
+        <v>2000</v>
       </c>
       <c r="E9">
-        <v>17</v>
+        <v>600</v>
       </c>
       <c r="F9">
         <v>5000</v>
       </c>
       <c r="G9" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="H9">
         <v>8</v>
@@ -802,22 +799,22 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10">
-        <v>9</v>
+        <v>2000</v>
       </c>
       <c r="E10">
-        <v>18</v>
+        <v>250</v>
       </c>
       <c r="F10">
         <v>5000</v>
       </c>
       <c r="G10" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="H10">
         <v>9</v>

</xml_diff>